<commit_message>
MaJ de laBDD complet
</commit_message>
<xml_diff>
--- a/01-Requetes SQL/fichier donnée excel.xlsx
+++ b/01-Requetes SQL/fichier donnée excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" firstSheet="15" activeTab="24"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" firstSheet="16" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2315,8 +2315,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2614,7 +2617,7 @@
   <dimension ref="A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2623,7 +2626,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
     </row>
@@ -2638,7 +2641,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2755,7 +2758,7 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -3121,7 +3124,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3154,7 +3157,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -3331,7 +3334,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3373,7 +3376,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -3448,7 +3451,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3499,7 +3502,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -3628,7 +3631,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3727,7 +3730,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -3971,7 +3974,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3995,7 +3998,7 @@
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
     </row>
@@ -4034,7 +4037,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4057,7 +4060,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
     </row>
@@ -4071,7 +4074,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4104,7 +4107,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -4137,7 +4140,7 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4161,7 +4164,7 @@
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
     </row>
@@ -4265,7 +4268,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4320,7 +4323,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
     </row>
@@ -4347,7 +4350,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4425,7 +4428,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -4480,7 +4483,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4549,7 +4552,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -4778,7 +4781,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4811,7 +4814,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -4836,7 +4839,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4896,7 +4899,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -4956,7 +4959,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4989,7 +4992,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -5126,7 +5129,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5207,7 +5210,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -5282,7 +5285,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5369,7 +5372,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -5528,7 +5531,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5561,7 +5564,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -5578,7 +5581,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5629,7 +5632,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -5652,7 +5655,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5685,7 +5688,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
     </row>
@@ -5712,7 +5715,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5757,7 +5760,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -6052,7 +6055,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6088,7 +6091,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -6137,7 +6140,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6179,7 +6182,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
     </row>
@@ -6193,7 +6196,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6226,7 +6229,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -6379,7 +6382,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6412,7 +6415,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -6445,7 +6448,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6577,7 +6580,7 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -7025,7 +7028,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7058,7 +7061,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -7219,7 +7222,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7279,7 +7282,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -7516,7 +7519,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7639,7 +7642,7 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">
@@ -8291,7 +8294,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8324,7 +8327,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>57234</v>
       </c>
       <c r="B4" t="s">

</xml_diff>